<commit_message>
include imported elec emissions
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
+++ b/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/ctrl-settings/biefie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\ctrl-settings\BIEfIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611D035E-B30F-3943-8580-0E58F028C670}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B5A04A-98EA-49EB-B89B-04C406AA1A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="22040" windowHeight="11840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -441,11 +441,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -453,42 +453,42 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -506,21 +506,23 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>